<commit_message>
(Re)add C12 to BOMs
</commit_message>
<xml_diff>
--- a/schematics/Uzebox-Omega/V1.1.1/Uzebox-Omega-1.1.1-BOM-DigiKey.xlsx
+++ b/schematics/Uzebox-Omega/V1.1.1/Uzebox-Omega-1.1.1-BOM-DigiKey.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Quantity</t>
   </si>
   <si>
-    <t xml:space="preserve">Uzebox Omega v1.1.1 Digi-Key BOM. Last updated 10th July 2025.</t>
+    <t xml:space="preserve">Uzebox Omega v1.1.1 Digi-Key BOM. Last updated 12th July 2025.</t>
   </si>
   <si>
     <t xml:space="preserve">2092-KMDGX-9S-N-ND</t>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">478-3192-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">CAP CER .10UF 50V 20% RADIAL        (C3,C4,C5,C6,C7)</t>
+    <t xml:space="preserve">CAP CER .10UF 50V 20% RADIAL        (C3,C4,C5,C6,C7,C12)</t>
   </si>
   <si>
     <t xml:space="preserve">478-5733-ND</t>
@@ -507,7 +507,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Remove 75R resistors from parts list, only 4x .10UF 50V caps required
</commit_message>
<xml_diff>
--- a/schematics/Uzebox-Omega/V1.1.1/Uzebox-Omega-1.1.1-BOM-DigiKey.xlsx
+++ b/schematics/Uzebox-Omega/V1.1.1/Uzebox-Omega-1.1.1-BOM-DigiKey.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Quantity</t>
   </si>
   <si>
-    <t xml:space="preserve">Uzebox Omega v1.1.1 Digi-Key BOM. Last updated 12th July 2025.</t>
+    <t xml:space="preserve">Uzebox Omega v1.1.1 Digi-Key BOM. Last updated 13th July 2025.</t>
   </si>
   <si>
     <t xml:space="preserve">2092-KMDGX-9S-N-ND</t>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">478-3192-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">CAP CER .10UF 50V 20% RADIAL        (C3,C4,C5,C6,C7,C12)</t>
+    <t xml:space="preserve">CAP CER .10UF 50V 20% RADIAL        (C3,C4,C5,C12)</t>
   </si>
   <si>
     <t xml:space="preserve">478-5733-ND</t>
@@ -507,7 +507,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Update Digikey BOM comments
</commit_message>
<xml_diff>
--- a/schematics/Uzebox-Omega/V1.1.1/Uzebox-Omega-1.1.1-BOM-DigiKey.xlsx
+++ b/schematics/Uzebox-Omega/V1.1.1/Uzebox-Omega-1.1.1-BOM-DigiKey.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Quantity</t>
   </si>
   <si>
-    <t xml:space="preserve">Uzebox Omega v1.1.1 Digi-Key BOM. Last updated 13th July 2025.</t>
+    <t xml:space="preserve">Uzebox Omega v1.1.1 Digi-Key BOM. Last updated 3rd September 2025.</t>
   </si>
   <si>
     <t xml:space="preserve">2092-KMDGX-9S-N-ND</t>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">CP-002A-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">CONN POWER JACK 2.1MM</t>
+    <t xml:space="preserve">CONN POWER JACK 2.1MM (7-12VDC)</t>
   </si>
   <si>
     <t xml:space="preserve">CP-1420-ND</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">3M5471-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">SOCKET IC OPEN FRAME 40POS .6"</t>
+    <t xml:space="preserve">SOCKET IC OPEN FRAME 40POS .6" (MCU)</t>
   </si>
   <si>
     <t xml:space="preserve">TS02-66-43-BK-100-LCR-D</t>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">399-ESK105M350AE3AA-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">CAP ELECT 1UF 50V VR RADIAL         (C16,C20)</t>
+    <t xml:space="preserve">CAP ALUM 1UF 20% 350V RADIAL TH         (C16,C20)</t>
   </si>
   <si>
     <t xml:space="preserve">478-3192-ND</t>
@@ -371,7 +371,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add SPI RAM and socket to DigiKey BOM
</commit_message>
<xml_diff>
--- a/schematics/Uzebox-Omega/V1.1.1/Uzebox-Omega-1.1.1-BOM-DigiKey.xlsx
+++ b/schematics/Uzebox-Omega/V1.1.1/Uzebox-Omega-1.1.1-BOM-DigiKey.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">Digi-Key Part Number</t>
   </si>
@@ -28,7 +28,40 @@
     <t xml:space="preserve">Quantity</t>
   </si>
   <si>
-    <t xml:space="preserve">Uzebox Omega v1.1.1 Digi-Key BOM. Last updated 3rd September 2025.</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Uzebox Omega v1.1.1 Digi-Key BOM. Last updated 5</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> September 2025.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">2092-KMDGX-9S-N-ND</t>
@@ -173,6 +206,18 @@
   </si>
   <si>
     <t xml:space="preserve">LED 3MM SHORT LENS GREEN DIFF       (LED1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AE9986-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN IC DIP SOCKET 8POS TIN        (U6)   - optional but recommended</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23LC1024-I/P-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC SRAM 1MBIT SPI/QUAD 8DIP         (U6)   - optional but recommended</t>
   </si>
 </sst>
 </file>
@@ -182,7 +227,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -215,6 +260,15 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <vertAlign val="superscript"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
@@ -368,10 +422,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -656,6 +710,28 @@
         <v>50</v>
       </c>
     </row>
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>